<commit_message>
se realizan correciones de los escenarios
</commit_message>
<xml_diff>
--- a/DATA_TEST_SAP.xlsx
+++ b/DATA_TEST_SAP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\juagudelo\pruebasUipath\Uipath\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3942E56-16AE-4CC1-AEA9-8F8E9DD0E9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814BA28B-CDC4-4537-ADF9-EF67B63D44A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2850" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRUEBAS" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1972" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="457">
   <si>
     <t>EJECUTADO</t>
   </si>
@@ -1327,82 +1327,76 @@
     <t>Caso 29-Ventas cliente 11- tipos de servicios</t>
   </si>
   <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>IVA MAYOR VALOR 4</t>
+  </si>
+  <si>
+    <t>IVA MAYOR VALOR 5</t>
+  </si>
+  <si>
+    <t>Se valida con documento base entrada en estado abierto,  que se genere la devolucion</t>
+  </si>
+  <si>
+    <t>ventas Cliente 2</t>
+  </si>
+  <si>
+    <t>Número de catálogo IC</t>
+  </si>
+  <si>
+    <t>Unidad de medida de inventario</t>
+  </si>
+  <si>
+    <t>Total (ML)</t>
+  </si>
+  <si>
+    <t>Sujeto a impuesto</t>
+  </si>
+  <si>
+    <t>Código de unidad de medida</t>
+  </si>
+  <si>
+    <t>País/región de origen</t>
+  </si>
+  <si>
+    <t>Precio de coste Centros de Costo</t>
+  </si>
+  <si>
+    <t>Centros de Costo</t>
+  </si>
+  <si>
+    <t>Unidad de Negocio</t>
+  </si>
+  <si>
+    <t>Precio de coste Unidad de Negocio</t>
+  </si>
+  <si>
+    <t>Marcadores lavables Norma, 12 unidades</t>
+  </si>
+  <si>
+    <t>$ 19,000.00</t>
+  </si>
+  <si>
+    <t>Regla plana de 30 cm, plástico</t>
+  </si>
+  <si>
+    <t>$ 8,000.00</t>
+  </si>
+  <si>
+    <t>TORNILLO ZINCADO 1</t>
+  </si>
+  <si>
+    <t>$ 5,000.00</t>
+  </si>
+  <si>
     <t>SI</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>ERROR</t>
-  </si>
-  <si>
-    <t>IVA MAYOR VALOR 4</t>
-  </si>
-  <si>
-    <t>Error no se esta generando retención</t>
-  </si>
-  <si>
-    <t>ERROR AL VALIDAR RETENCIONES -&gt; no genero retencion</t>
-  </si>
-  <si>
-    <t>IVA MAYOR VALOR 5</t>
-  </si>
-  <si>
-    <t>Se valida con documento base entrada en estado abierto,  que se genere la devolucion</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Error validacion Fila 1: no coincide codigo de indicador de impuesto o base de impuesto --&gt; indicador de impuesto :ACRE Base de impuesto-168,000.00 N</t>
-  </si>
-  <si>
-    <t>ventas Cliente 2</t>
-  </si>
-  <si>
-    <t>Número de catálogo IC</t>
-  </si>
-  <si>
-    <t>Unidad de medida de inventario</t>
-  </si>
-  <si>
-    <t>Total (ML)</t>
-  </si>
-  <si>
-    <t>Sujeto a impuesto</t>
-  </si>
-  <si>
-    <t>Código de unidad de medida</t>
-  </si>
-  <si>
-    <t>País/región de origen</t>
-  </si>
-  <si>
-    <t>Precio de coste Centros de Costo</t>
-  </si>
-  <si>
-    <t>Centros de Costo</t>
-  </si>
-  <si>
-    <t>Unidad de Negocio</t>
-  </si>
-  <si>
-    <t>Precio de coste Unidad de Negocio</t>
-  </si>
-  <si>
-    <t>Marcadores lavables Norma, 12 unidades</t>
-  </si>
-  <si>
-    <t>$ 19,000.00</t>
-  </si>
-  <si>
-    <t>Regla plana de 30 cm, plástico</t>
-  </si>
-  <si>
-    <t>$ 8,000.00</t>
-  </si>
-  <si>
-    <t>TORNILLO ZINCADO 1</t>
-  </si>
-  <si>
-    <t>$ 5,000.00</t>
+    <t>A81:C86</t>
+  </si>
+  <si>
+    <t>Caso 28-Ventas cliente 10</t>
   </si>
 </sst>
 </file>
@@ -1412,7 +1406,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1442,8 +1436,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1471,12 +1471,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1528,7 +1522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1567,7 +1561,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1890,9 +1886,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21:B26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2065,9 +2061,11 @@
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="2" t="s">
         <v>433</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>454</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="2" t="s">
@@ -2192,9 +2190,11 @@
       </c>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="25" t="s">
+      <c r="A3" s="2" t="s">
         <v>433</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>454</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="2" t="s">
@@ -2319,11 +2319,13 @@
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="25" t="s">
+      <c r="A4" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="B4" s="20" t="s">
+        <v>454</v>
+      </c>
+      <c r="C4" s="13"/>
       <c r="D4" s="2" t="s">
         <v>276</v>
       </c>
@@ -2447,14 +2449,12 @@
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>433</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>437</v>
-      </c>
+        <v>454</v>
+      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>277</v>
       </c>
@@ -2578,14 +2578,12 @@
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="B6" s="20" t="s">
         <v>433</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>437</v>
-      </c>
+      <c r="B6" s="16" t="s">
+        <v>454</v>
+      </c>
+      <c r="C6" s="13"/>
       <c r="D6" s="2" t="s">
         <v>279</v>
       </c>
@@ -2707,16 +2705,14 @@
         <v>275</v>
       </c>
     </row>
-    <row r="7" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="B7" s="20" t="s">
         <v>433</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>438</v>
-      </c>
+      <c r="B7" s="16" t="s">
+        <v>454</v>
+      </c>
+      <c r="C7" s="13"/>
       <c r="D7" s="2" t="s">
         <v>281</v>
       </c>
@@ -2840,10 +2836,10 @@
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B8" s="20" t="s">
         <v>433</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>454</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="2" t="s">
@@ -2969,10 +2965,10 @@
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B9" s="20" t="s">
         <v>433</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>454</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="2" t="s">
@@ -3096,10 +3092,10 @@
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B10" s="20" t="s">
         <v>433</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>454</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="2" t="s">
@@ -3225,10 +3221,10 @@
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B11" s="20" t="s">
         <v>433</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>454</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="2" t="s">
@@ -3354,14 +3350,14 @@
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B12" s="20" t="s">
         <v>433</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>454</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>304</v>
@@ -3420,7 +3416,7 @@
       <c r="W12" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="X12" s="2">
+      <c r="X12" s="26">
         <v>4320</v>
       </c>
       <c r="Y12" s="2">
@@ -3483,17 +3479,17 @@
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B13" s="20" t="s">
         <v>433</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>454</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>261</v>
@@ -3612,10 +3608,10 @@
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B14" s="26" t="s">
         <v>433</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>454</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="2" t="s">
@@ -3741,10 +3737,10 @@
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B15" s="26" t="s">
         <v>433</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>454</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="2" t="s">
@@ -3870,10 +3866,10 @@
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B16" s="20" t="s">
         <v>433</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>454</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="2" t="s">
@@ -3999,10 +3995,10 @@
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B17" s="26" t="s">
         <v>433</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>454</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="2" t="s">
@@ -4126,10 +4122,10 @@
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B18" s="26" t="s">
         <v>433</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>454</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="2" t="s">
@@ -4212,10 +4208,10 @@
         <v>275</v>
       </c>
       <c r="AE18" s="11">
-        <v>44609.443761574075</v>
+        <v>44819.065810185188</v>
       </c>
       <c r="AF18" s="11">
-        <v>44609.444293981483</v>
+        <v>44819.066342592596</v>
       </c>
       <c r="AG18" s="2" t="s">
         <v>314</v>
@@ -4253,10 +4249,10 @@
     </row>
     <row r="19" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B19" s="26" t="s">
         <v>433</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>454</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="2" t="s">
@@ -4339,10 +4335,10 @@
         <v>275</v>
       </c>
       <c r="AE19" s="11">
-        <v>44609.447708333333</v>
+        <v>44825.747546296298</v>
       </c>
       <c r="AF19" s="11">
-        <v>44609.448599537034</v>
+        <v>44825.748124999998</v>
       </c>
       <c r="AG19" s="2" t="s">
         <v>314</v>
@@ -4380,10 +4376,10 @@
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>433</v>
+        <v>454</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="2" t="s">
@@ -4507,10 +4503,10 @@
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>3</v>
+        <v>433</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>454</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="2" t="s">
@@ -4634,10 +4630,10 @@
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>3</v>
+        <v>433</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>454</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="2" t="s">
@@ -4761,10 +4757,10 @@
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>3</v>
+        <v>433</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>454</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="2" t="s">
@@ -4890,10 +4886,10 @@
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>3</v>
+        <v>433</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>454</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="2" t="s">
@@ -5019,10 +5015,10 @@
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>3</v>
+        <v>433</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>454</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="2" t="s">
@@ -5148,10 +5144,10 @@
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>3</v>
+        <v>433</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>454</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="2" t="s">
@@ -5276,9 +5272,11 @@
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="26" t="s">
+      <c r="A27" s="2" t="s">
         <v>433</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>454</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="2" t="s">
@@ -5339,7 +5337,7 @@
         <v>275</v>
       </c>
       <c r="W27" s="9">
-        <v>149838.14000000001</v>
+        <v>38610.78</v>
       </c>
       <c r="X27" s="9" t="s">
         <v>275</v>
@@ -5404,10 +5402,10 @@
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="B28" s="26" t="s">
         <v>433</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>454</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="2" t="s">
@@ -5533,10 +5531,10 @@
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B29" s="16" t="s">
         <v>433</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>454</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="2" t="s">
@@ -5660,16 +5658,14 @@
         <v>275</v>
       </c>
     </row>
-    <row r="30" spans="1:43" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="B30" s="16" t="s">
         <v>433</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>441</v>
-      </c>
+      <c r="B30" s="25" t="s">
+        <v>454</v>
+      </c>
+      <c r="C30" s="13"/>
       <c r="D30" s="2" t="s">
         <v>427</v>
       </c>
@@ -5919,7 +5915,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="X33" s="2">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="34" spans="7:24" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
         <v>420</v>
       </c>
@@ -5927,7 +5928,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:24" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
         <v>421</v>
       </c>
@@ -5946,8 +5947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C89B120-B27A-4858-A0DC-4A8AB9E97B35}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:Q39"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6041,15 +6042,15 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="29" t="s">
         <v>370</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -6080,15 +6081,15 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="29" t="s">
         <v>394</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -6147,15 +6148,15 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="29" t="s">
         <v>401</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -6214,15 +6215,15 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="29" t="s">
         <v>429</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -6282,7 +6283,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -6290,7 +6291,7 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
@@ -6299,7 +6300,7 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="F36" t="s">
         <v>8</v>
@@ -6311,31 +6312,31 @@
         <v>10</v>
       </c>
       <c r="I36" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="J36" t="s">
         <v>61</v>
       </c>
       <c r="K36" t="s">
+        <v>441</v>
+      </c>
+      <c r="L36" t="s">
+        <v>442</v>
+      </c>
+      <c r="M36" t="s">
+        <v>443</v>
+      </c>
+      <c r="N36" t="s">
+        <v>444</v>
+      </c>
+      <c r="O36" t="s">
+        <v>445</v>
+      </c>
+      <c r="P36" t="s">
         <v>446</v>
       </c>
-      <c r="L36" t="s">
+      <c r="Q36" t="s">
         <v>447</v>
-      </c>
-      <c r="M36" t="s">
-        <v>448</v>
-      </c>
-      <c r="N36" t="s">
-        <v>449</v>
-      </c>
-      <c r="O36" t="s">
-        <v>450</v>
-      </c>
-      <c r="P36" t="s">
-        <v>451</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -6343,13 +6344,13 @@
         <v>1018</v>
       </c>
       <c r="C37" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="D37">
         <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="H37" t="s">
         <v>363</v>
@@ -6375,13 +6376,13 @@
         <v>1019</v>
       </c>
       <c r="C38" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="D38">
         <v>5</v>
       </c>
       <c r="F38" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="H38" t="s">
         <v>363</v>
@@ -6407,13 +6408,13 @@
         <v>1020</v>
       </c>
       <c r="C39" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="D39">
         <v>6</v>
       </c>
       <c r="F39" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="H39" t="s">
         <v>363</v>
@@ -9551,10 +9552,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2850B6B2-9175-479E-99DE-8AB5102C7A56}">
-  <dimension ref="A1:AB77"/>
+  <dimension ref="A1:AB86"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="I71" sqref="I71"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9565,10 +9566,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>376</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="30"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -9715,11 +9716,11 @@
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="30" t="s">
         <v>392</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -9817,11 +9818,11 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="30" t="s">
         <v>403</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -9884,11 +9885,11 @@
       <c r="K43" s="4"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="30" t="s">
         <v>402</v>
       </c>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
@@ -9961,11 +9962,11 @@
       <c r="K51" s="4"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
+      <c r="A54" s="30" t="s">
         <v>425</v>
       </c>
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
@@ -10034,11 +10035,20 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="28" t="s">
+      <c r="A62" s="30" t="s">
         <v>426</v>
       </c>
-      <c r="B62" s="28"/>
-      <c r="C62" s="28"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="30"/>
+      <c r="F62" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
@@ -10050,6 +10060,15 @@
       <c r="C63" s="2" t="s">
         <v>373</v>
       </c>
+      <c r="F63" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
@@ -10059,6 +10078,15 @@
         <v>152</v>
       </c>
       <c r="C64" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="H64" s="2" t="s">
         <v>423</v>
       </c>
       <c r="K64" s="4"/>
@@ -10068,10 +10096,19 @@
         <v>396</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>371</v>
+        <v>194</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>423</v>
+        <v>404</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>424</v>
       </c>
       <c r="K65" s="4"/>
     </row>
@@ -10080,22 +10117,40 @@
         <v>396</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F66" s="2">
+        <v>0</v>
+      </c>
+      <c r="G66" s="2">
+        <v>0</v>
+      </c>
+      <c r="H66" s="2">
+        <v>0</v>
+      </c>
+      <c r="K66" s="4"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="K66" s="4"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="C67" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G67" s="2">
         <v>0</v>
       </c>
-      <c r="B67" s="2">
-        <v>0</v>
-      </c>
-      <c r="C67" s="2">
-        <v>0</v>
+      <c r="H67" s="2" t="s">
+        <v>423</v>
       </c>
       <c r="K67" s="4"/>
     </row>
@@ -10103,19 +10158,19 @@
       <c r="A68" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>423</v>
+      <c r="B68" s="2">
+        <v>0</v>
+      </c>
+      <c r="C68" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="28" t="s">
+      <c r="A70" s="30" t="s">
         <v>432</v>
       </c>
-      <c r="B70" s="28"/>
-      <c r="C70" s="28"/>
+      <c r="B70" s="30"/>
+      <c r="C70" s="30"/>
       <c r="K70" s="4"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -10197,8 +10252,85 @@
         <v>57</v>
       </c>
     </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="30" t="s">
+        <v>456</v>
+      </c>
+      <c r="B80" s="30"/>
+      <c r="C80" s="30"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="B82" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C82" s="28">
+        <v>-200000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="B83" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="C83" s="28">
+        <v>-200000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="B84" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="C84" s="28">
+        <v>-3000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="B85" s="27">
+        <v>0</v>
+      </c>
+      <c r="C85" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="B86" s="27">
+        <v>0</v>
+      </c>
+      <c r="C86" s="27">
+        <v>0</v>
+      </c>
+      <c r="E86" t="s">
+        <v>455</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A80:C80"/>
     <mergeCell ref="A70:C70"/>
     <mergeCell ref="A62:C62"/>
     <mergeCell ref="A54:C54"/>

</xml_diff>